<commit_message>
MABG:09.08.22 - Bug en error de correo de union
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -109,7 +109,7 @@
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>85573</x:t>
+    <x:t>85815</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,8 +158,32 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="34">
+  <x:cellStyleXfs count="42">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -609,7 +633,7 @@
       <x:selection activeCell="A17" sqref="A17 A17:A17"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="131.37" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="134.2125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="9" customWidth="1"/>
     <x:col min="2" max="2" width="132" style="9" customWidth="1"/>

</xml_diff>

<commit_message>
JLV:25.08.2022: Descarga de documentos Word
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:loext="http://schemas.libreoffice.org/" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Robots\uipath\ACTFINAN-GBO_Descarga\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Robots\uipath\RPA3 - OCEANS\ACTFINAN-GBO_Descarga_Server\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF58F032-1027-48B6-9251-6FE8D5A71230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F45BA4-DC20-4EC0-A2E9-AE50FA2A9F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Input_Parameters" sheetId="1" r:id="rId1"/>
@@ -103,13 +103,13 @@
     <x:t>ExcelDescargas</x:t>
   </x:si>
   <x:si>
-    <x:t>D:\Git\Robots\uipath\ACTFINAN-GBO_Descarga\Descargar.xlsx</x:t>
+    <x:t>D:\Git\Robots\uipath\RPA3 - OCEANS\ACTFINAN-GBO_Descarga_Server\Descargar.xlsx</x:t>
   </x:si>
   <x:si>
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>85815</x:t>
+    <x:t>86890</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,157 +158,168 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="42">
+  <x:cellStyleXfs count="46">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="10">
+  <x:cellXfs count="9">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -630,15 +641,15 @@
   <x:dimension ref="A1:Z1048520"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <x:selection activeCell="A17" sqref="A17 A17:A17"/>
+      <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="134.2125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="156.204063" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="36.140625" style="9" customWidth="1"/>
-    <x:col min="2" max="2" width="132" style="9" customWidth="1"/>
-    <x:col min="3" max="3" width="50.425781" style="6" customWidth="1"/>
-    <x:col min="4" max="26" width="8.710938" style="6" customWidth="1"/>
+    <x:col min="1" max="1" width="36.140625" style="6" customWidth="1"/>
+    <x:col min="2" max="2" width="132" style="6" customWidth="1"/>
+    <x:col min="3" max="3" width="50.425781" style="5" customWidth="1"/>
+    <x:col min="4" max="26" width="8.710938" style="5" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -676,109 +687,109 @@
       <x:c r="Z1" s="8" t="s"/>
     </x:row>
     <x:row r="2" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="s">
+      <x:c r="A2" s="6" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="B2" s="9" t="s">
+      <x:c r="B2" s="6" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="9" t="s">
+      <x:c r="A3" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B3" s="9" t="s">
+      <x:c r="B3" s="6" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="9" t="s">
+      <x:c r="A4" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="B4" s="9" t="s">
+      <x:c r="B4" s="6" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="9" t="s">
+      <x:c r="A5" s="6" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B5" s="9" t="s">
+      <x:c r="B5" s="6" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="9" t="s">
+      <x:c r="A6" s="6" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B6" s="9" t="s">
+      <x:c r="B6" s="6" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="9" t="s">
+      <x:c r="A7" s="6" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B7" s="9" t="s">
+      <x:c r="B7" s="6" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="9" t="s">
+      <x:c r="A8" s="6" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="B8" s="9" t="s">
+      <x:c r="B8" s="6" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="9" t="s">
+      <x:c r="A9" s="6" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="B9" s="9" t="s">
+      <x:c r="B9" s="6" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C9" s="6" t="s">
+      <x:c r="C9" s="5" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="9" t="s">
+      <x:c r="A10" s="6" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="B10" s="9" t="s">
+      <x:c r="B10" s="6" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="9" t="s">
+      <x:c r="A11" s="6" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B11" s="9" t="s">
+      <x:c r="B11" s="6" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="9" t="s">
+      <x:c r="A12" s="6" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B12" s="9" t="s">
+      <x:c r="B12" s="6" t="s">
         <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="9" t="s">
+      <x:c r="A13" s="6" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B13" s="9" t="s">
+      <x:c r="B13" s="6" t="s">
         <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:26" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="6" t="s">
+      <x:c r="A14" s="5" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B14" s="9" t="s">
+      <x:c r="B14" s="6" t="s">
         <x:v>29</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
JLV:25.08.2022: Cambios en la descarga del RPA2
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -5,10 +5,10 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Robots\uipath\RPA3 - OCEANS\ACTFINAN-GBO_Descarga_Server\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Robots\uipath\RPA2 - OCEANS - Subida a HRC\ACTFINAN-GBO_Descarga_Server\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F45BA4-DC20-4EC0-A2E9-AE50FA2A9F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F79AFAF-D837-43A1-894A-B4C6CB8AE615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -103,13 +103,13 @@
     <x:t>ExcelDescargas</x:t>
   </x:si>
   <x:si>
-    <x:t>D:\Git\Robots\uipath\RPA3 - OCEANS\ACTFINAN-GBO_Descarga_Server\Descargar.xlsx</x:t>
+    <x:t>D:\Git\Robots\uipath\RPA2 - OCEANS - Subida a HRC\ACTFINAN-GBO_Descarga_Server\Descargar.xlsx</x:t>
   </x:si>
   <x:si>
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>86890</x:t>
+    <x:t>86688</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,33 +158,9 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="46">
+  <x:cellStyleXfs count="38">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -644,7 +620,7 @@
       <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="156.204063" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="153.361563" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="6" customWidth="1"/>
     <x:col min="2" max="2" width="132" style="6" customWidth="1"/>

</xml_diff>

<commit_message>
MABG : MEJORAS EN LA UNION
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -109,7 +109,7 @@
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>87134</x:t>
+    <x:t>88685</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,9 +158,81 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="48">
+  <x:cellStyleXfs count="72">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -650,7 +722,7 @@
       <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="156.914688" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="165.442188" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="6" customWidth="1"/>
     <x:col min="2" max="2" width="132" style="6" customWidth="1"/>

</xml_diff>

<commit_message>
MABG:09.09.09-BUGS- Correccion de Filtro, para no bajar
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -109,7 +109,7 @@
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>88685</x:t>
+    <x:t>91905</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,9 +158,75 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="72">
+  <x:cellStyleXfs count="94">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -722,7 +788,7 @@
       <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="165.442188" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="173.259063" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="6" customWidth="1"/>
     <x:col min="2" max="2" width="132" style="6" customWidth="1"/>

</xml_diff>

<commit_message>
MABG:14.10.22 - Subir a git Descargas Oceans
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -109,7 +109,7 @@
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>88685</x:t>
+    <x:t>104885</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,9 +158,177 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="62">
+  <x:cellStyleXfs count="118">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -692,7 +860,7 @@
       <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="161.889063" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="181.786563" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="6" customWidth="1"/>
     <x:col min="2" max="2" width="132" style="6" customWidth="1"/>

</xml_diff>

<commit_message>
MABG:07.11.22 - Excel Descrgas y Union
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -109,7 +109,7 @@
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>107968</x:t>
+    <x:t>113444</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,9 +158,189 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="148">
+  <x:cellStyleXfs count="208">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -950,7 +1130,7 @@
       <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="192.445938" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="213.764688" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="6" customWidth="1"/>
     <x:col min="2" max="2" width="132" style="6" customWidth="1"/>

</xml_diff>

<commit_message>
MABG: 10_11_22 - TODO OK
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -109,7 +109,7 @@
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>113444</x:t>
+    <x:t>114784</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,9 +158,57 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="208">
+  <x:cellStyleXfs count="224">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -1130,7 +1178,7 @@
       <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="213.764688" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="219.449688" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="6" customWidth="1"/>
     <x:col min="2" max="2" width="132" style="6" customWidth="1"/>

</xml_diff>

<commit_message>
MABG:11.11.22 - TODO OK
</commit_message>
<xml_diff>
--- a/Data/Input/Config.xlsx
+++ b/Data/Input/Config.xlsx
@@ -109,7 +109,7 @@
     <x:t>LineasIQY</x:t>
   </x:si>
   <x:si>
-    <x:t>114784</x:t>
+    <x:t>115260</x:t>
   </x:si>
   <x:si>
     <x:t>mailRecipient</x:t>
@@ -158,9 +158,21 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="224">
+  <x:cellStyleXfs count="228">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -1178,7 +1190,7 @@
       <x:selection activeCell="B12" sqref="B12 B12:B12"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="219.449688" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="220.870938" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="36.140625" style="6" customWidth="1"/>
     <x:col min="2" max="2" width="132" style="6" customWidth="1"/>

</xml_diff>